<commit_message>
correction des decimaux du prix unitaire d'un article
</commit_message>
<xml_diff>
--- a/test_factures_sage100.xlsx
+++ b/test_factures_sage100.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Facture_003_ERREURS" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Avoir_001" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Facture_COMPLEXE" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Test_TVA_Cases" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -486,7 +487,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>850000</v>
+        <v>849999.5</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -496,13 +497,11 @@
           <t>pcs</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>TVA</t>
-        </is>
+      <c r="G20" t="n">
+        <v>18</v>
       </c>
       <c r="H20" t="n">
-        <v>850000</v>
+        <v>849999.5</v>
       </c>
     </row>
     <row r="21">
@@ -517,7 +516,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>25000</v>
+        <v>24750.25</v>
       </c>
       <c r="E21" t="n">
         <v>2</v>
@@ -527,13 +526,11 @@
           <t>pcs</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>TVA</t>
-        </is>
+      <c r="G21" t="n">
+        <v>18</v>
       </c>
       <c r="H21" t="n">
-        <v>50000</v>
+        <v>49500.5</v>
       </c>
     </row>
   </sheetData>
@@ -630,7 +627,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>650</v>
+        <v>649.75</v>
       </c>
       <c r="E20" t="n">
         <v>50</v>
@@ -640,13 +637,11 @@
           <t>litres</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>TVA</t>
-        </is>
+      <c r="G20" t="n">
+        <v>9</v>
       </c>
       <c r="H20" t="n">
-        <v>32500</v>
+        <v>32487.5</v>
       </c>
     </row>
   </sheetData>
@@ -740,10 +735,8 @@
           <t>pcs</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>TVX</t>
-        </is>
+      <c r="G20" t="n">
+        <v>99</v>
       </c>
       <c r="H20" t="n">
         <v>100000</v>
@@ -836,7 +829,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>-150000</v>
+        <v>-149999.99</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -846,13 +839,11 @@
           <t>pcs</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>TVA</t>
-        </is>
+      <c r="G20" t="n">
+        <v>18</v>
       </c>
       <c r="H20" t="n">
-        <v>-150000</v>
+        <v>-149999.99</v>
       </c>
     </row>
   </sheetData>
@@ -935,7 +926,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>100000</v>
+        <v>99999.75</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -945,13 +936,11 @@
           <t>service</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>TVA</t>
-        </is>
+      <c r="G20" t="n">
+        <v>18</v>
       </c>
       <c r="H20" t="n">
-        <v>100000</v>
+        <v>99999.75</v>
       </c>
     </row>
     <row r="21">
@@ -966,7 +955,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>500000</v>
+        <v>499850.5</v>
       </c>
       <c r="E21" t="n">
         <v>3</v>
@@ -976,13 +965,11 @@
           <t>pcs</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>TVA</t>
-        </is>
+      <c r="G21" t="n">
+        <v>18</v>
       </c>
       <c r="H21" t="n">
-        <v>1500000</v>
+        <v>1499551.5</v>
       </c>
     </row>
     <row r="22">
@@ -997,7 +984,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>75000</v>
+        <v>74999.25</v>
       </c>
       <c r="E22" t="n">
         <v>8</v>
@@ -1007,13 +994,11 @@
           <t>heures</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>TVAB</t>
-        </is>
+      <c r="G22" t="n">
+        <v>9</v>
       </c>
       <c r="H22" t="n">
-        <v>600000</v>
+        <v>599994</v>
       </c>
     </row>
     <row r="23">
@@ -1028,7 +1013,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>200000</v>
+        <v>199950.75</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -1038,13 +1023,11 @@
           <t>service</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>TVA</t>
-        </is>
+      <c r="G23" t="n">
+        <v>18</v>
       </c>
       <c r="H23" t="n">
-        <v>200000</v>
+        <v>199950.75</v>
       </c>
     </row>
     <row r="24">
@@ -1059,7 +1042,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>350000</v>
+        <v>349999</v>
       </c>
       <c r="E24" t="n">
         <v>2</v>
@@ -1069,13 +1052,189 @@
           <t>licence</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>TVAC</t>
-        </is>
-      </c>
       <c r="H24" t="n">
-        <v>700000</v>
+        <v>699998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:H23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TEST001</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CLI_TEST</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1234567T</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>45512</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CLIENT TEST TVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PROD_18</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Produit avec TVA 18%</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>100.5</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>18</v>
+      </c>
+      <c r="H20" t="n">
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PROD_9</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Produit avec TVA 9%</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>200.75</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>9</v>
+      </c>
+      <c r="H21" t="n">
+        <v>200.75</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>PROD_0</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Produit avec TVA 0%</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>150</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>PROD_VIDE</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Produit avec cellule TVA vide</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>300.25</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>pcs</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>300.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>